<commit_message>
Add ecran modifié ...
</commit_message>
<xml_diff>
--- a/TNR_JDD/JDD.RT.ART.xlsx
+++ b/TNR_JDD/JDD.RT.ART.xlsx
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="297">
   <si>
     <t>Date</t>
   </si>
@@ -792,13 +792,22 @@
     <t>ORG.RT.ART.001.LEC.01.........</t>
   </si>
   <si>
-    <t>ARTICLE GENERIQUE</t>
+    <t>ARTICLE D'ETE</t>
   </si>
   <si>
-    <t>TEXTE ARTICLE GENERIQUE</t>
+    <t>TEXTE ARTICLE D'ETE</t>
   </si>
   <si>
     <t>CCO.RT.ART.001.LEC.01</t>
+  </si>
+  <si>
+    <t>VENTE VALORISEE</t>
+  </si>
+  <si>
+    <t>ORG.RT.ART.001.LEC.01</t>
+  </si>
+  <si>
+    <t>FANNY</t>
   </si>
   <si>
     <t>RT.ART.001.MAJ.01</t>
@@ -823,6 +832,9 @@
   </si>
   <si>
     <t>RT.ART.001.REC.01</t>
+  </si>
+  <si>
+    <t>ARTICLE GENERIQUE</t>
   </si>
   <si>
     <t>RT.ART*001*ID_CODART</t>
@@ -912,7 +924,7 @@
     <t>REF RT.ART.001.LEC.01</t>
   </si>
   <si>
-    <t>DESIGNATION FOURNISSEUR ARTICLE GENERIQUE</t>
+    <t>DESIGNATION FOURNISSEUR ARTICLE D'ETE</t>
   </si>
   <si>
     <t>TEXTE1 RT.ART.001.LEC.01</t>
@@ -989,6 +1001,30 @@
     <t>//div[@id='DVID_NUMDOC1']</t>
   </si>
   <si>
+    <t>tab_Article</t>
+  </si>
+  <si>
+    <t>$TAB$ID_CODART</t>
+  </si>
+  <si>
+    <t>tab_ArticleSelected</t>
+  </si>
+  <si>
+    <t>$TABSELECTED$ID_CODART</t>
+  </si>
+  <si>
+    <t>input_Filtre_Grille</t>
+  </si>
+  <si>
+    <t>$FILTREGRILLE$ID_CODART</t>
+  </si>
+  <si>
+    <t>td_Grille</t>
+  </si>
+  <si>
+    <t>$TDGRILLE$2$ID_CODART</t>
+  </si>
+  <si>
     <t>Champ</t>
   </si>
 </sst>
@@ -1000,7 +1036,7 @@
     <numFmt numFmtId="164" formatCode="D/M/YYYY"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1112,6 +1148,11 @@
       <sz val="9.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="16">
@@ -1243,7 +1284,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="88">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1469,6 +1510,15 @@
     </xf>
     <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="15" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -7880,7 +7930,7 @@
         <v>227</v>
       </c>
       <c r="K11" s="55" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="L11" s="19" t="s">
         <v>228</v>
@@ -7932,7 +7982,7 @@
       </c>
       <c r="AH11" s="56"/>
       <c r="AI11" s="57" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="AJ11" s="19" t="s">
         <v>197</v>
@@ -7952,20 +8002,28 @@
       <c r="AO11" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="AP11" s="19"/>
-      <c r="AQ11" s="19"/>
-      <c r="AR11" s="19"/>
-      <c r="AS11" s="19"/>
+      <c r="AP11" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="AQ11" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="AR11" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="AS11" s="19" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="54" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B12" s="55" t="s">
         <v>183</v>
       </c>
       <c r="C12" s="59" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>184</v>
@@ -7981,23 +8039,23 @@
         <v>200</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="K12" s="55" t="s">
         <v>190</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="N12" s="56"/>
       <c r="O12" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="P12" s="56"/>
       <c r="Q12" s="56"/>
@@ -8032,10 +8090,10 @@
         <v>195</v>
       </c>
       <c r="AF12" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="AG12" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="AH12" s="56"/>
       <c r="AI12" s="57" t="s">
@@ -8066,13 +8124,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="54" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B13" s="55" t="s">
         <v>183</v>
       </c>
       <c r="C13" s="59" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D13" s="62"/>
       <c r="E13" s="63"/>
@@ -8119,13 +8177,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="54" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B14" s="55" t="s">
         <v>183</v>
       </c>
       <c r="C14" s="59" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D14" s="64"/>
       <c r="E14" s="63"/>
@@ -37211,18 +37269,18 @@
         <v>1000.0</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="54" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B12" s="60">
         <v>1001.0</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -40537,10 +40595,10 @@
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D2" s="48" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E2" s="48"/>
       <c r="F2" s="48"/>
@@ -40656,7 +40714,7 @@
         <v>178</v>
       </c>
       <c r="J5" s="49" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="K5" s="49"/>
       <c r="L5" s="49"/>
@@ -40724,7 +40782,7 @@
         <v>182</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>184</v>
@@ -40736,13 +40794,13 @@
         <v>186</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="K7" s="19">
         <v>10.0</v>
@@ -40755,13 +40813,13 @@
       </c>
       <c r="N7" s="56"/>
       <c r="O7" s="19" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="P7" s="19" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="R7" s="72" t="s">
         <v>186</v>
@@ -40782,7 +40840,7 @@
         <v>45292.0</v>
       </c>
       <c r="X7" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="Y7" s="55" t="s">
         <v>195</v>
@@ -40808,7 +40866,7 @@
         <v>198</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>208</v>
@@ -40820,13 +40878,13 @@
         <v>186</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="K8" s="19">
         <v>20.0</v>
@@ -40839,13 +40897,13 @@
       </c>
       <c r="N8" s="56"/>
       <c r="O8" s="19" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="P8" s="19" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="R8" s="72" t="s">
         <v>186</v>
@@ -40866,7 +40924,7 @@
         <v>45292.0</v>
       </c>
       <c r="X8" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="Y8" s="55" t="s">
         <v>195</v>
@@ -40892,7 +40950,7 @@
         <v>207</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>208</v>
@@ -40904,13 +40962,13 @@
         <v>186</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="K9" s="19">
         <v>30.0</v>
@@ -40923,13 +40981,13 @@
       </c>
       <c r="N9" s="56"/>
       <c r="O9" s="19" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="R9" s="72" t="s">
         <v>186</v>
@@ -40950,7 +41008,7 @@
         <v>45292.0</v>
       </c>
       <c r="X9" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="Y9" s="55" t="s">
         <v>195</v>
@@ -40976,7 +41034,7 @@
         <v>216</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>208</v>
@@ -40988,13 +41046,13 @@
         <v>186</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="K10" s="19">
         <v>40.0</v>
@@ -41007,13 +41065,13 @@
       </c>
       <c r="N10" s="56"/>
       <c r="O10" s="19" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="R10" s="72" t="s">
         <v>186</v>
@@ -41034,7 +41092,7 @@
         <v>45292.0</v>
       </c>
       <c r="X10" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="Y10" s="55" t="s">
         <v>195</v>
@@ -41060,7 +41118,7 @@
         <v>224</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>208</v>
@@ -41072,13 +41130,13 @@
         <v>186</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K11" s="19">
         <v>50.0</v>
@@ -41091,13 +41149,13 @@
       </c>
       <c r="N11" s="56"/>
       <c r="O11" s="19" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="R11" s="72" t="s">
         <v>186</v>
@@ -41118,7 +41176,7 @@
         <v>45292.0</v>
       </c>
       <c r="X11" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="Y11" s="61" t="s">
         <v>195</v>
@@ -41135,16 +41193,16 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="54" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B12" s="55" t="s">
         <v>183</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>184</v>
@@ -41156,13 +41214,13 @@
         <v>186</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="K12" s="19">
         <v>100.0</v>
@@ -41175,13 +41233,13 @@
       </c>
       <c r="N12" s="56"/>
       <c r="O12" s="19" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="R12" s="72" t="s">
         <v>186</v>
@@ -41219,13 +41277,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="54" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B13" s="55" t="s">
         <v>183</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D13" s="74"/>
       <c r="E13" s="74"/>
@@ -41255,13 +41313,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="54" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B14" s="55" t="s">
         <v>183</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D14" s="74"/>
       <c r="E14" s="74"/>
@@ -53440,10 +53498,10 @@
       </c>
       <c r="B2" s="77"/>
       <c r="C2" s="49" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3">
@@ -53552,13 +53610,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="54" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B12" s="55" t="s">
         <v>183</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D12" s="55">
         <v>1006.0</v>
@@ -53566,13 +53624,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="54" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B13" s="55" t="s">
         <v>183</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D13" s="55">
         <v>1007.0</v>
@@ -53580,13 +53638,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="54" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B14" s="55" t="s">
         <v>183</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D14" s="55">
         <v>1008.0</v>
@@ -56794,30 +56852,70 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="83" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B1" s="84" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C1" s="84" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="31" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="3" ht="12.75" customHeight="1"/>
-    <row r="4" ht="12.75" customHeight="1"/>
-    <row r="5" ht="12.75" customHeight="1"/>
-    <row r="6" ht="12.75" customHeight="1"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1">
+      <c r="A3" s="85" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" s="86" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" s="86" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" s="85" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" s="86" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="86" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" s="85" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" s="85" t="s">
+        <v>292</v>
+      </c>
+      <c r="C5" s="87" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1">
+      <c r="A6" s="85" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6" s="85" t="s">
+        <v>294</v>
+      </c>
+      <c r="C6" s="87" t="s">
+        <v>295</v>
+      </c>
+    </row>
     <row r="7" ht="12.75" customHeight="1"/>
     <row r="8" ht="12.75" customHeight="1"/>
     <row r="9" ht="12.75" customHeight="1"/>
@@ -57844,7 +57942,7 @@
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="41"/>
       <c r="B1" s="44" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>

</xml_diff>

<commit_message>
Ajout new JDDKW $UPD$val$newval
Ajout dans CheckTypeInDATA
Ajout dans PREJDDFile
</commit_message>
<xml_diff>
--- a/TNR_JDD/JDD.RT.ART.xlsx
+++ b/TNR_JDD/JDD.RT.ART.xlsx
@@ -49,14 +49,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgU18AhfFE4vEJcTNdHzaFmp8F61A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mi9bK+4XNxLweasw6rVEiPyul92GA=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="298">
   <si>
     <t>Date</t>
   </si>
@@ -3379,7 +3379,9 @@
       <c r="C30" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="21"/>
+      <c r="D30" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E30" s="19" t="s">
         <v>29</v>
       </c>
@@ -3395,7 +3397,9 @@
       <c r="C31" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="21"/>
+      <c r="D31" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E31" s="19" t="s">
         <v>29</v>
       </c>
@@ -3411,7 +3415,9 @@
       <c r="C32" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="21"/>
+      <c r="D32" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E32" s="19" t="s">
         <v>29</v>
       </c>
@@ -7083,13 +7089,13 @@
       <c r="AA1" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="AB1" s="45" t="s">
+      <c r="AB1" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="AC1" s="45" t="s">
+      <c r="AC1" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="AD1" s="45" t="s">
+      <c r="AD1" s="46" t="s">
         <v>95</v>
       </c>
       <c r="AE1" s="46" t="s">
@@ -7184,15 +7190,9 @@
       <c r="Y2" s="49"/>
       <c r="Z2" s="49"/>
       <c r="AA2" s="49"/>
-      <c r="AB2" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC2" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD2" s="51" t="s">
-        <v>28</v>
-      </c>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
       <c r="AE2" s="49"/>
       <c r="AF2" s="49"/>
       <c r="AG2" s="49"/>
@@ -7523,14 +7523,14 @@
       <c r="AA7" s="60">
         <v>0.0</v>
       </c>
-      <c r="AB7" s="19">
-        <v>100.0</v>
-      </c>
-      <c r="AC7" s="19">
-        <v>200.0</v>
-      </c>
-      <c r="AD7" s="19">
-        <v>300.0</v>
+      <c r="AB7" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC7" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD7" s="60" t="s">
+        <v>187</v>
       </c>
       <c r="AE7" s="60" t="s">
         <v>196</v>
@@ -7638,14 +7638,14 @@
       <c r="AA8" s="60">
         <v>0.0</v>
       </c>
-      <c r="AB8" s="19">
-        <v>110.0</v>
-      </c>
-      <c r="AC8" s="19">
-        <v>210.0</v>
-      </c>
-      <c r="AD8" s="19">
-        <v>310.0</v>
+      <c r="AB8" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC8" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD8" s="60" t="s">
+        <v>187</v>
       </c>
       <c r="AE8" s="60" t="s">
         <v>196</v>
@@ -7753,14 +7753,14 @@
       <c r="AA9" s="60">
         <v>0.0</v>
       </c>
-      <c r="AB9" s="19">
-        <v>120.0</v>
-      </c>
-      <c r="AC9" s="19">
-        <v>220.0</v>
-      </c>
-      <c r="AD9" s="19">
-        <v>320.0</v>
+      <c r="AB9" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC9" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD9" s="60" t="s">
+        <v>187</v>
       </c>
       <c r="AE9" s="60" t="s">
         <v>196</v>
@@ -7868,14 +7868,14 @@
       <c r="AA10" s="60">
         <v>0.0</v>
       </c>
-      <c r="AB10" s="19">
-        <v>130.0</v>
-      </c>
-      <c r="AC10" s="19">
-        <v>230.0</v>
-      </c>
-      <c r="AD10" s="19">
-        <v>330.0</v>
+      <c r="AB10" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC10" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD10" s="60" t="s">
+        <v>187</v>
       </c>
       <c r="AE10" s="60" t="s">
         <v>196</v>
@@ -7983,14 +7983,14 @@
       <c r="AA11" s="60">
         <v>0.0</v>
       </c>
-      <c r="AB11" s="19">
-        <v>140.0</v>
-      </c>
-      <c r="AC11" s="19">
-        <v>240.0</v>
-      </c>
-      <c r="AD11" s="19">
-        <v>340.0</v>
+      <c r="AB11" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC11" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD11" s="60" t="s">
+        <v>187</v>
       </c>
       <c r="AE11" s="60" t="s">
         <v>196</v>
@@ -8106,14 +8106,14 @@
       <c r="AA12" s="60">
         <v>0.0</v>
       </c>
-      <c r="AB12" s="19">
-        <v>150.0</v>
-      </c>
-      <c r="AC12" s="19">
-        <v>250.0</v>
-      </c>
-      <c r="AD12" s="19">
-        <v>350.0</v>
+      <c r="AB12" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC12" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD12" s="60" t="s">
+        <v>187</v>
       </c>
       <c r="AE12" s="60" t="s">
         <v>196</v>
@@ -8277,6 +8277,9 @@
       <c r="Y15" s="71"/>
       <c r="Z15" s="71"/>
       <c r="AA15" s="71"/>
+      <c r="AB15" s="71"/>
+      <c r="AC15" s="71"/>
+      <c r="AD15" s="71"/>
       <c r="AE15" s="71"/>
       <c r="AH15" s="61"/>
       <c r="AK15" s="71"/>
@@ -8304,6 +8307,9 @@
       <c r="Y16" s="71"/>
       <c r="Z16" s="71"/>
       <c r="AA16" s="71"/>
+      <c r="AB16" s="71"/>
+      <c r="AC16" s="71"/>
+      <c r="AD16" s="71"/>
       <c r="AE16" s="71"/>
       <c r="AH16" s="61"/>
       <c r="AK16" s="71"/>

</xml_diff>

<commit_message>
ajout de setDebugLevel et setDebugDeph à ajouter où on veut
Par exemple dans les script _CHECK PREREQUIS et _CREATE PREJDD IN DB
</commit_message>
<xml_diff>
--- a/TNR_JDD/JDD.RT.ART.xlsx
+++ b/TNR_JDD/JDD.RT.ART.xlsx
@@ -28,28 +28,6 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="D19">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAA0bKFVE8
-Nicolas HUC    (2023-07-06 06:58:03)
-@jean-marc.lafarge-ext@apave.com Question à élucider
-_Attribuée à Jean-Marc LAFARGE_
-------
-ID#AAAA1Nt11Zw
-Jean-Marc LAFARGE    (2023-07-18 09:38:55)
-@nicolas.huc@apave.com
-_Réattribué à Nicolas HUC_
-------
-ID#AAAA1Nt11Z0
-Jean-Marc LAFARGE    (2023-07-18 09:40:56)
-rien à voir avec la notion de matricule obligatoire, si le champ est à O, lors d'une sortie de stock, l'article en question est automatiquement ajouté dans la table ART_EQU de l'équipement concerné (fonction héritée de Mainta SI).
-------
-ID#AAAA1Nt11Z4
-Jean-Marc LAFARGE    (2023-07-18 09:41:03)
-@nicolas.huc@apave.com</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="D59">
       <text>
         <t xml:space="preserve">======
@@ -60,20 +38,29 @@
 ------
 ID#AAAA1Nt11Zs
 Jean-Marc LAFARGE    (2023-07-18 09:38:41)
-représente le coefficient quantité de commande d'un article chez un fournisseur. Mis à jour lors du changement d'unité article dans le catalogue</t>
+représente le coefficient quantité de commande d'un article chez un fournisseur. Mis à jour lors du changement d'unité article dans le catalogue
+------
+ID#AAAA1ZE6IcU
+Jean-Marc LAFARGE    (2023-07-19 05:50:34)
+@nicolas.huc@apave.com
+_Réattribué à Nicolas HUC_
+------
+ID#AAAA1ZOAlf4
+Nicolas HUC    (2023-07-19 05:54:05)
+Cette rubrique est-elle utilisée en dehors de cette table ? Je ne vois pas l'intérêt puisque le coefficient est défini au niveau de l'unité-même (Cela me semble même risqué de le stocker au niveau de ART_FOU).</t>
       </text>
     </comment>
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miz/Jn5muFVKSFlTwfSEffhMxbi7w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miOuwlrD90DL9ShMxGMy1k4GwuZ0g=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="308">
   <si>
     <t>Date</t>
   </si>
@@ -299,7 +286,7 @@
     <t>ST_CRENOM</t>
   </si>
   <si>
-    <t>OBSOLETE ? Question MOE</t>
+    <t>Apprentissage automatique de la nomenclature</t>
   </si>
   <si>
     <t>NU_DEL</t>
@@ -512,6 +499,9 @@
     <t>Coefficient</t>
   </si>
   <si>
+    <t>OBSOLETE ? Question MOE</t>
+  </si>
+  <si>
     <t>???</t>
   </si>
   <si>
@@ -688,6 +678,9 @@
     <t>N</t>
   </si>
   <si>
+    <t>O</t>
+  </si>
+  <si>
     <t>$DATETIMESYS</t>
   </si>
   <si>
@@ -833,9 +826,6 @@
   </si>
   <si>
     <t>CCO.UPD.RT.ART.001.MAJ.01</t>
-  </si>
-  <si>
-    <t>O</t>
   </si>
   <si>
     <t>RT.ART.001.SUP.01</t>
@@ -3213,14 +3203,12 @@
         <v>68</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="21" t="s">
-        <v>69</v>
-      </c>
+      <c r="D19" s="21"/>
       <c r="E19" s="19" t="s">
         <v>29</v>
       </c>
@@ -3920,19 +3908,19 @@
         <v>37</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="E59" s="36" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F59" s="34"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
       <c r="A60" s="31" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C60" s="31" t="s">
         <v>57</v>
@@ -3945,10 +3933,10 @@
     </row>
     <row r="61" ht="12.75" customHeight="1">
       <c r="A61" s="31" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C61" s="31" t="s">
         <v>57</v>
@@ -3961,10 +3949,10 @@
     </row>
     <row r="62" ht="12.75" customHeight="1">
       <c r="A62" s="31" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C62" s="31" t="s">
         <v>57</v>
@@ -3980,13 +3968,13 @@
         <v>87</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C63" s="31" t="s">
         <v>37</v>
       </c>
       <c r="D63" s="37" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E63" s="19" t="s">
         <v>29</v>
@@ -3995,16 +3983,16 @@
     </row>
     <row r="64">
       <c r="A64" s="31" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C64" s="31" t="s">
         <v>62</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E64" s="19" t="s">
         <v>29</v>
@@ -4016,7 +4004,7 @@
         <v>76</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C65" s="31" t="s">
         <v>78</v>
@@ -4031,10 +4019,10 @@
     </row>
     <row r="66" ht="12.75" customHeight="1">
       <c r="A66" s="31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B66" s="31" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C66" s="31" t="s">
         <v>78</v>
@@ -4047,10 +4035,10 @@
     </row>
     <row r="67" ht="12.75" customHeight="1">
       <c r="A67" s="31" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B67" s="31" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C67" s="31" t="s">
         <v>78</v>
@@ -4063,10 +4051,10 @@
     </row>
     <row r="68" ht="12.75" customHeight="1">
       <c r="A68" s="31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B68" s="31" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C68" s="31" t="s">
         <v>78</v>
@@ -4079,10 +4067,10 @@
     </row>
     <row r="69" ht="12.75" customHeight="1">
       <c r="A69" s="31" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B69" s="31" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C69" s="31" t="s">
         <v>65</v>
@@ -4138,7 +4126,7 @@
         <v>113</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C72" s="31" t="s">
         <v>78</v>
@@ -4156,7 +4144,7 @@
         <v>115</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C73" s="31" t="s">
         <v>78</v>
@@ -4171,10 +4159,10 @@
     </row>
     <row r="74" ht="12.75" customHeight="1">
       <c r="A74" s="26" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B74" s="27" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C74" s="39"/>
       <c r="D74" s="26">
@@ -4221,10 +4209,10 @@
     </row>
     <row r="77" ht="12.75" customHeight="1">
       <c r="A77" s="31" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C77" s="32" t="s">
         <v>37</v>
@@ -7163,19 +7151,19 @@
         <v>115</v>
       </c>
       <c r="AO1" s="48" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AP1" s="48" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AQ1" s="48" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AR1" s="48" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AS1" s="48" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2">
@@ -7192,7 +7180,7 @@
       <c r="G2" s="49"/>
       <c r="H2" s="49"/>
       <c r="I2" s="49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J2" s="49"/>
       <c r="K2" s="49"/>
@@ -7205,9 +7193,7 @@
       <c r="P2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="50" t="s">
-        <v>28</v>
-      </c>
+      <c r="Q2" s="50"/>
       <c r="R2" s="50" t="s">
         <v>28</v>
       </c>
@@ -7247,7 +7233,7 @@
     </row>
     <row r="3">
       <c r="A3" s="49" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
@@ -7290,27 +7276,27 @@
       <c r="AN3" s="49"/>
       <c r="AO3" s="49"/>
       <c r="AP3" s="49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AQ3" s="49" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AR3" s="49" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AS3" s="49" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
       <c r="D4" s="49"/>
       <c r="E4" s="50" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F4" s="49"/>
       <c r="G4" s="49"/>
@@ -7355,39 +7341,39 @@
     </row>
     <row r="5">
       <c r="A5" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B5" s="51"/>
       <c r="C5" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="51"/>
       <c r="G5" s="51"/>
       <c r="H5" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I5" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J5" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K5" s="51" t="s">
+        <v>182</v>
+      </c>
+      <c r="L5" s="51" t="s">
         <v>181</v>
       </c>
-      <c r="L5" s="51" t="s">
-        <v>180</v>
-      </c>
       <c r="M5" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N5" s="51"/>
       <c r="O5" s="51" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P5" s="51"/>
       <c r="Q5" s="51"/>
@@ -7401,48 +7387,48 @@
       <c r="Y5" s="51"/>
       <c r="Z5" s="51"/>
       <c r="AA5" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AB5" s="51"/>
       <c r="AC5" s="51"/>
       <c r="AD5" s="51"/>
       <c r="AE5" s="51"/>
       <c r="AF5" s="51" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AG5" s="51" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AH5" s="51"/>
       <c r="AI5" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AJ5" s="51" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AK5" s="51"/>
       <c r="AL5" s="51"/>
       <c r="AM5" s="51"/>
       <c r="AN5" s="51"/>
       <c r="AO5" s="52" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AP5" s="49" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AQ5" s="49" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AR5" s="49" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AS5" s="49" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="53" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B6" s="53"/>
       <c r="C6" s="53"/>
@@ -7491,113 +7477,115 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="55" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F7" s="57"/>
       <c r="G7" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K7" s="56" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="N7" s="57"/>
       <c r="O7" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="P7" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q7" s="57"/>
+        <v>190</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>198</v>
+      </c>
       <c r="R7" s="57"/>
       <c r="S7" s="57"/>
       <c r="T7" s="57"/>
       <c r="U7" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="V7" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="W7" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="X7" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y7" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z7" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA7" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB7" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC7" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD7" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE7" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF7" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="V7" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="W7" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="X7" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="Y7" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z7" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA7" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="AB7" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AC7" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AD7" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AE7" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="AF7" s="19" t="s">
-        <v>196</v>
-      </c>
       <c r="AG7" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AH7" s="57"/>
       <c r="AI7" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ7" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK7" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AL7" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AM7" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="AJ7" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="AK7" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="AL7" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="AM7" s="56" t="s">
+      <c r="AN7" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AO7" s="19" t="s">
         <v>197</v>
-      </c>
-      <c r="AN7" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AO7" s="19" t="s">
-        <v>196</v>
       </c>
       <c r="AP7" s="19"/>
       <c r="AQ7" s="19"/>
@@ -7606,113 +7594,115 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="55" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F8" s="57"/>
       <c r="G8" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="K8" s="56" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="N8" s="57"/>
       <c r="O8" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="P8" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q8" s="57"/>
+        <v>190</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>197</v>
+      </c>
       <c r="R8" s="57"/>
       <c r="S8" s="57"/>
       <c r="T8" s="57"/>
       <c r="U8" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="V8" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="W8" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="X8" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y8" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z8" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA8" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB8" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC8" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD8" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE8" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF8" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="V8" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="W8" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="X8" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="Y8" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z8" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA8" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="AB8" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AC8" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AD8" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AE8" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="AF8" s="19" t="s">
-        <v>196</v>
-      </c>
       <c r="AG8" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AH8" s="57"/>
       <c r="AI8" s="59" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="AJ8" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK8" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="AK8" s="56" t="s">
-        <v>198</v>
-      </c>
       <c r="AL8" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AM8" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="AN8" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AO8" s="19" t="s">
         <v>197</v>
-      </c>
-      <c r="AN8" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AO8" s="19" t="s">
-        <v>196</v>
       </c>
       <c r="AP8" s="19"/>
       <c r="AQ8" s="19"/>
@@ -7721,113 +7711,115 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="55" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F9" s="57"/>
       <c r="G9" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="K9" s="56" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="N9" s="57"/>
       <c r="O9" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="P9" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q9" s="57"/>
+        <v>190</v>
+      </c>
+      <c r="Q9" s="19" t="s">
+        <v>198</v>
+      </c>
       <c r="R9" s="57"/>
       <c r="S9" s="57"/>
       <c r="T9" s="57"/>
       <c r="U9" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="V9" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="W9" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="X9" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y9" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z9" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA9" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB9" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC9" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD9" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE9" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF9" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="V9" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="W9" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="X9" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="Y9" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z9" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA9" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="AB9" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AC9" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AD9" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AE9" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="AF9" s="19" t="s">
-        <v>196</v>
-      </c>
       <c r="AG9" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AH9" s="57"/>
       <c r="AI9" s="59" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="AJ9" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK9" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="AK9" s="56" t="s">
-        <v>198</v>
-      </c>
       <c r="AL9" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AM9" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="AN9" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AO9" s="19" t="s">
         <v>197</v>
-      </c>
-      <c r="AN9" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AO9" s="19" t="s">
-        <v>196</v>
       </c>
       <c r="AP9" s="19"/>
       <c r="AQ9" s="19"/>
@@ -7836,113 +7828,115 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="55" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F10" s="57"/>
       <c r="G10" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="K10" s="60" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="N10" s="57"/>
       <c r="O10" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="P10" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q10" s="57"/>
+        <v>190</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>197</v>
+      </c>
       <c r="R10" s="57"/>
       <c r="S10" s="57"/>
       <c r="T10" s="57"/>
       <c r="U10" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="V10" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="W10" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="X10" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y10" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z10" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA10" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB10" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC10" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD10" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE10" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF10" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="V10" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="W10" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="X10" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="Y10" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z10" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA10" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="AB10" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AC10" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AD10" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AE10" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="AF10" s="19" t="s">
-        <v>196</v>
-      </c>
       <c r="AG10" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AH10" s="57"/>
       <c r="AI10" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ10" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK10" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AL10" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AM10" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="AJ10" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="AK10" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="AL10" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="AM10" s="56" t="s">
+      <c r="AN10" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AO10" s="19" t="s">
         <v>197</v>
-      </c>
-      <c r="AN10" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AO10" s="19" t="s">
-        <v>196</v>
       </c>
       <c r="AP10" s="19"/>
       <c r="AQ10" s="19"/>
@@ -7951,236 +7945,240 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="55" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C11" s="61" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E11" s="62">
         <v>1000.0</v>
       </c>
       <c r="F11" s="57"/>
       <c r="G11" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="K11" s="56" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="N11" s="57"/>
       <c r="O11" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="P11" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q11" s="57"/>
+        <v>190</v>
+      </c>
+      <c r="Q11" s="19" t="s">
+        <v>198</v>
+      </c>
       <c r="R11" s="57"/>
       <c r="S11" s="57"/>
       <c r="T11" s="57"/>
       <c r="U11" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="V11" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="W11" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="X11" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y11" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="Z11" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA11" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB11" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC11" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD11" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE11" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF11" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="V11" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="W11" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="X11" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="Y11" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z11" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA11" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="AB11" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AC11" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AD11" s="56" t="s">
-        <v>189</v>
-      </c>
-      <c r="AE11" s="56" t="s">
-        <v>198</v>
-      </c>
-      <c r="AF11" s="19" t="s">
-        <v>196</v>
-      </c>
       <c r="AG11" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AH11" s="57"/>
       <c r="AI11" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ11" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK11" s="63" t="s">
+        <v>200</v>
+      </c>
+      <c r="AL11" s="63" t="s">
+        <v>200</v>
+      </c>
+      <c r="AM11" s="63" t="s">
         <v>199</v>
       </c>
-      <c r="AJ11" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="AK11" s="63" t="s">
-        <v>198</v>
-      </c>
-      <c r="AL11" s="63" t="s">
-        <v>198</v>
-      </c>
-      <c r="AM11" s="63" t="s">
+      <c r="AN11" s="63" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO11" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="AN11" s="63" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO11" s="19" t="s">
-        <v>196</v>
-      </c>
       <c r="AP11" s="19" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AQ11" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="AR11" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="AS11" s="19" t="s">
         <v>238</v>
-      </c>
-      <c r="AR11" s="19" t="s">
-        <v>239</v>
-      </c>
-      <c r="AS11" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="55" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C12" s="61" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E12" s="62">
         <v>1001.0</v>
       </c>
       <c r="F12" s="57"/>
       <c r="G12" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="K12" s="56" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="N12" s="57"/>
       <c r="O12" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="P12" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q12" s="57"/>
+        <v>190</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>197</v>
+      </c>
       <c r="R12" s="57"/>
       <c r="S12" s="57"/>
       <c r="T12" s="57"/>
       <c r="U12" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="V12" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="W12" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="X12" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Y12" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="Z12" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AA12" s="19" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AB12" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AC12" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AD12" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AE12" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF12" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="AF12" s="19" t="s">
-        <v>246</v>
-      </c>
       <c r="AG12" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="AH12" s="57"/>
       <c r="AI12" s="59" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="AJ12" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK12" s="63" t="s">
         <v>200</v>
       </c>
-      <c r="AK12" s="63" t="s">
-        <v>198</v>
-      </c>
       <c r="AL12" s="63" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AM12" s="63" t="s">
+        <v>199</v>
+      </c>
+      <c r="AN12" s="63" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO12" s="19" t="s">
         <v>197</v>
-      </c>
-      <c r="AN12" s="63" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO12" s="19" t="s">
-        <v>196</v>
       </c>
       <c r="AP12" s="19"/>
       <c r="AQ12" s="19"/>
@@ -8189,13 +8187,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="55" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D13" s="58"/>
       <c r="E13" s="64"/>
@@ -8242,13 +8240,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="55" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D14" s="65"/>
       <c r="E14" s="64"/>
@@ -36151,98 +36149,98 @@
     </row>
     <row r="3">
       <c r="A3" s="49" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
     </row>
     <row r="4">
       <c r="A4" s="49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C4" s="49"/>
     </row>
     <row r="5">
       <c r="A5" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B5" s="51"/>
       <c r="C5" s="49"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="53" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B6" s="53"/>
       <c r="C6" s="53"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="55" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="55" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="55" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="55" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="55" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B11" s="62">
         <v>1000.0</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="55" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B12" s="62">
         <v>1001.0</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
@@ -39509,34 +39507,34 @@
         <v>138</v>
       </c>
       <c r="O1" s="71" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P1" s="71" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Q1" s="71" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R1" s="71" t="s">
         <v>87</v>
       </c>
       <c r="S1" s="71" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="T1" s="46" t="s">
         <v>76</v>
       </c>
       <c r="U1" s="46" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="V1" s="71" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="W1" s="71" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="X1" s="71" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Y1" s="46" t="s">
         <v>110</v>
@@ -39557,10 +39555,10 @@
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
@@ -39591,7 +39589,7 @@
     </row>
     <row r="3">
       <c r="A3" s="50" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B3" s="49"/>
       <c r="C3" s="49"/>
@@ -39623,7 +39621,7 @@
     </row>
     <row r="4">
       <c r="A4" s="50" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
@@ -39655,33 +39653,33 @@
     </row>
     <row r="5">
       <c r="A5" s="50" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="50" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D5" s="50" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G5" s="51"/>
       <c r="H5" s="50"/>
       <c r="I5" s="50" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J5" s="50" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="K5" s="50"/>
       <c r="L5" s="50"/>
       <c r="M5" s="50" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N5" s="51"/>
       <c r="O5" s="50"/>
@@ -39694,7 +39692,7 @@
       <c r="V5" s="50"/>
       <c r="W5" s="50"/>
       <c r="X5" s="50" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="Y5" s="51"/>
       <c r="Z5" s="51"/>
@@ -39703,7 +39701,7 @@
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="72" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B6" s="53"/>
       <c r="C6" s="53"/>
@@ -39735,34 +39733,34 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="55" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F7" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7" s="56" t="s">
         <v>190</v>
       </c>
-      <c r="G7" s="56" t="s">
-        <v>189</v>
-      </c>
       <c r="H7" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="K7" s="19">
         <v>10.0</v>
@@ -39775,13 +39773,13 @@
       </c>
       <c r="N7" s="57"/>
       <c r="O7" s="19" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="P7" s="19" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="R7" s="19">
         <v>0.0</v>
@@ -39790,10 +39788,10 @@
         <v>0.0</v>
       </c>
       <c r="T7" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="U7" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="V7" s="73">
         <v>44927.0</v>
@@ -39802,51 +39800,51 @@
         <v>45292.0</v>
       </c>
       <c r="X7" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="Y7" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="Z7" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AA7" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AB7" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="55" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F8" s="59" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G8" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="K8" s="19">
         <v>20.0</v>
@@ -39859,13 +39857,13 @@
       </c>
       <c r="N8" s="57"/>
       <c r="O8" s="19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P8" s="19" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="R8" s="19">
         <v>0.0</v>
@@ -39874,10 +39872,10 @@
         <v>0.0</v>
       </c>
       <c r="T8" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="U8" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="V8" s="73">
         <v>44927.0</v>
@@ -39886,51 +39884,51 @@
         <v>45292.0</v>
       </c>
       <c r="X8" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="Y8" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="Z8" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AA8" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AB8" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="55" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G9" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="K9" s="19">
         <v>30.0</v>
@@ -39943,13 +39941,13 @@
       </c>
       <c r="N9" s="57"/>
       <c r="O9" s="19" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="Q9" s="19" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="R9" s="19">
         <v>0.0</v>
@@ -39958,10 +39956,10 @@
         <v>0.0</v>
       </c>
       <c r="T9" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="U9" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="V9" s="73">
         <v>44927.0</v>
@@ -39970,51 +39968,51 @@
         <v>45292.0</v>
       </c>
       <c r="X9" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="Y9" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="Z9" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AA9" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AB9" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="55" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="K10" s="19">
         <v>40.0</v>
@@ -40027,13 +40025,13 @@
       </c>
       <c r="N10" s="57"/>
       <c r="O10" s="19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="R10" s="19">
         <v>0.0</v>
@@ -40042,10 +40040,10 @@
         <v>0.0</v>
       </c>
       <c r="T10" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="U10" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="V10" s="73">
         <v>44927.0</v>
@@ -40054,51 +40052,51 @@
         <v>45292.0</v>
       </c>
       <c r="X10" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="Y10" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="Z10" s="56" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AA10" s="56" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AB10" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="55" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F11" s="59" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K11" s="19">
         <v>50.0</v>
@@ -40111,13 +40109,13 @@
       </c>
       <c r="N11" s="57"/>
       <c r="O11" s="19" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="R11" s="19">
         <v>0.0</v>
@@ -40126,10 +40124,10 @@
         <v>0.0</v>
       </c>
       <c r="T11" s="63" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="U11" s="63" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="V11" s="73">
         <v>44927.0</v>
@@ -40138,51 +40136,51 @@
         <v>45292.0</v>
       </c>
       <c r="X11" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="Y11" s="63" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="Z11" s="63" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AA11" s="63" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AB11" s="63" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="55" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G12" s="56" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K12" s="19">
         <v>100.0</v>
@@ -40195,13 +40193,13 @@
       </c>
       <c r="N12" s="57"/>
       <c r="O12" s="19" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Q12" s="19" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="R12" s="19">
         <v>0.0</v>
@@ -40210,10 +40208,10 @@
         <v>0.0</v>
       </c>
       <c r="T12" s="63" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="U12" s="63" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="V12" s="73">
         <v>44562.0</v>
@@ -40222,30 +40220,30 @@
         <v>45658.0</v>
       </c>
       <c r="X12" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Y12" s="63" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="Z12" s="63" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AA12" s="63" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AB12" s="63" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="55" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D13" s="74"/>
       <c r="E13" s="74"/>
@@ -40275,13 +40273,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="55" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D14" s="74"/>
       <c r="E14" s="74"/>
@@ -52420,7 +52418,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="76" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>25</v>
@@ -52429,7 +52427,7 @@
         <v>31</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E1" s="45"/>
       <c r="F1" s="45"/>
@@ -52460,15 +52458,15 @@
       </c>
       <c r="B2" s="77"/>
       <c r="C2" s="50" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="77" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B3" s="78"/>
       <c r="C3" s="79"/>
@@ -52476,7 +52474,7 @@
     </row>
     <row r="4">
       <c r="A4" s="77" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" s="78"/>
       <c r="C4" s="79"/>
@@ -52484,17 +52482,17 @@
     </row>
     <row r="5">
       <c r="A5" s="77" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B5" s="78"/>
       <c r="C5" s="80" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D5" s="51"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="81" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B6" s="54"/>
       <c r="C6" s="82"/>
@@ -52502,13 +52500,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="55" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D7" s="56">
         <v>1001.0</v>
@@ -52516,13 +52514,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="55" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D8" s="56">
         <v>1002.0</v>
@@ -52530,13 +52528,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="55" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D9" s="56">
         <v>1003.0</v>
@@ -52544,13 +52542,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="55" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D10" s="56">
         <v>1004.0</v>
@@ -52558,13 +52556,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="55" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D11" s="56">
         <v>1005.0</v>
@@ -52572,13 +52570,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="55" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D12" s="56">
         <v>1006.0</v>
@@ -52586,13 +52584,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="55" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D13" s="56">
         <v>1007.0</v>
@@ -52600,13 +52598,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="55" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D14" s="56">
         <v>1008.0</v>
@@ -55814,68 +55812,68 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="83" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B1" s="84" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C1" s="84" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="31" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="85" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B3" s="86" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C3" s="86" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="85" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B4" s="86" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C4" s="86" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="85" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="85" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B6" s="85" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C6" s="87" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
@@ -56904,7 +56902,7 @@
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="42"/>
       <c r="B1" s="45" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C1" s="45"/>
       <c r="D1" s="45"/>
@@ -56939,25 +56937,25 @@
     </row>
     <row r="3">
       <c r="A3" s="49" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B3" s="49"/>
     </row>
     <row r="4">
       <c r="A4" s="49" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" s="49"/>
     </row>
     <row r="5">
       <c r="A5" s="49" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B5" s="49"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="53" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B6" s="53"/>
     </row>

</xml_diff>